<commit_message>
Update the TA with the new world names
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/TAsetup.xlsx
+++ b/AD-EYE/TA/TAsetup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3A175E-9268-498E-AAAA-A5C0EA9156AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327FC5DB-E694-45F1-94F1-75F538DF7D40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30870" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>hostname</t>
   </si>
   <si>
-    <t>192.168.1.91</t>
-  </si>
-  <si>
     <t>adeye03u</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>ROS_folder</t>
+  </si>
+  <si>
+    <t>192.168.1.131</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +406,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -435,10 +435,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -446,7 +446,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>